<commit_message>
reorganized mf gos by
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/GO/organizing/MN_GO.xlsx
+++ b/analyses/T7-incubations/unipept/GO/organizing/MN_GO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="organizingCC" sheetId="1" state="visible" r:id="rId2"/>
@@ -6730,8 +6730,8 @@
   </sheetPr>
   <dimension ref="A1:L344"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15895,8 +15895,8 @@
   </sheetPr>
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K31" activeCellId="0" sqref="K31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>